<commit_message>
#15 i dont remember, sorry
</commit_message>
<xml_diff>
--- a/data/DocProperties/DocProperties_filled.xlsx
+++ b/data/DocProperties/DocProperties_filled.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WORK\InCore\PyMarkup4CS\data\DocProperties\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C97E26-B281-4CC8-A2BC-D9F6085531F2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8B2D4E-5FDB-4D69-8929-D7A23711899E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="6660" windowHeight="1785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2004" uniqueCount="1975">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2007" uniqueCount="1978">
   <si>
     <t>Name</t>
   </si>
@@ -16795,6 +16795,16 @@
   </si>
   <si>
     <t>Код перевіряє кількість об'єктів страхування в програмі з кодом "250"; якщо їх більше одного — повертає текст "Згідно з Додатком 2 до Договору", інакше — повертає страхову ставку з точністю до чотирьох знаків.</t>
+  </si>
+  <si>
+    <t>InsurerName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">__Result = "Вітаємо, " + __Product.Insurer.Face.Firstname + " " + __Product.Insurer.Face.Secondname;
+</t>
+  </si>
+  <si>
+    <t>ім'я страхувальника</t>
   </si>
 </sst>
 </file>
@@ -17163,10 +17173,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C952"/>
+  <dimension ref="A1:C953"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B93" sqref="B93"/>
+    <sheetView tabSelected="1" topLeftCell="A952" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C963" sqref="C963"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25028,7 +25038,7 @@
         <v>1877</v>
       </c>
     </row>
-    <row r="945" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+    <row r="945" spans="1:3" ht="195" x14ac:dyDescent="0.25">
       <c r="A945" t="s">
         <v>1878</v>
       </c>
@@ -25036,7 +25046,7 @@
         <v>1879</v>
       </c>
     </row>
-    <row r="946" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+    <row r="946" spans="1:3" ht="195" x14ac:dyDescent="0.25">
       <c r="A946" t="s">
         <v>1880</v>
       </c>
@@ -25044,7 +25054,7 @@
         <v>1881</v>
       </c>
     </row>
-    <row r="947" spans="1:2" ht="300" x14ac:dyDescent="0.25">
+    <row r="947" spans="1:3" ht="300" x14ac:dyDescent="0.25">
       <c r="A947" t="s">
         <v>1882</v>
       </c>
@@ -25052,7 +25062,7 @@
         <v>1883</v>
       </c>
     </row>
-    <row r="948" spans="1:2" ht="300" x14ac:dyDescent="0.25">
+    <row r="948" spans="1:3" ht="300" x14ac:dyDescent="0.25">
       <c r="A948" t="s">
         <v>1884</v>
       </c>
@@ -25060,7 +25070,7 @@
         <v>1885</v>
       </c>
     </row>
-    <row r="949" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+    <row r="949" spans="1:3" ht="195" x14ac:dyDescent="0.25">
       <c r="A949" t="s">
         <v>1886</v>
       </c>
@@ -25068,7 +25078,7 @@
         <v>1887</v>
       </c>
     </row>
-    <row r="950" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+    <row r="950" spans="1:3" ht="195" x14ac:dyDescent="0.25">
       <c r="A950" t="s">
         <v>1888</v>
       </c>
@@ -25076,7 +25086,7 @@
         <v>1889</v>
       </c>
     </row>
-    <row r="951" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+    <row r="951" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A951" t="s">
         <v>1890</v>
       </c>
@@ -25084,12 +25094,23 @@
         <v>1891</v>
       </c>
     </row>
-    <row r="952" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+    <row r="952" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A952" t="s">
         <v>1892</v>
       </c>
       <c r="B952" s="1" t="s">
         <v>1893</v>
+      </c>
+    </row>
+    <row r="953" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A953" t="s">
+        <v>1975</v>
+      </c>
+      <c r="B953" s="5" t="s">
+        <v>1976</v>
+      </c>
+      <c r="C953" s="1" t="s">
+        <v>1977</v>
       </c>
     </row>
   </sheetData>

</xml_diff>